<commit_message>
VCF-SV: prototype - wip
</commit_message>
<xml_diff>
--- a/modules/VCF-SV/proto/proto-BOM.xlsx
+++ b/modules/VCF-SV/proto/proto-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCF-SV\proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{51597728-C5C0-434F-A033-39AA5B28B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B63DDA5-0637-4DEE-ADCC-DDBCD1031316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="2670" windowWidth="19380" windowHeight="11820"/>
+    <workbookView xWindow="1290" yWindow="2325" windowWidth="19380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proto-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="100">
   <si>
     <t>Ref</t>
   </si>
@@ -137,15 +150,6 @@
   </si>
   <si>
     <t>Capacitor - Film</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Conn_01x09</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x09, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
     <t>R1 R14</t>
@@ -334,7 +338,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1180,11 +1184,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1265,9 +1269,12 @@
       <c r="B2">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
       <c r="E2">
-        <f>B2-C2-D2</f>
-        <v>4</v>
+        <f>MAX(B2-C2-D2,0)</f>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1285,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E22" si="0">B3-C3-D3</f>
+        <f t="shared" ref="E3:E21" si="0">MAX(B3-C3-D3,0)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1323,9 +1330,12 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -1341,9 +1351,12 @@
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -1359,9 +1372,12 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
@@ -1375,95 +1391,125 @@
         <v>39</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>40</v>
       </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>45</v>
-      </c>
-      <c r="J8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
       </c>
       <c r="M8" t="s">
         <v>28</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
         <v>52</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>45</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" t="s">
-        <v>48</v>
       </c>
       <c r="M9" t="s">
         <v>28</v>
       </c>
       <c r="N9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1471,389 +1517,401 @@
         <v>53</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" t="s">
         <v>45</v>
-      </c>
-      <c r="J10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" t="s">
-        <v>48</v>
       </c>
       <c r="M10" t="s">
         <v>28</v>
       </c>
       <c r="N10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" t="s">
         <v>44</v>
       </c>
-      <c r="I11" t="s">
+      <c r="L11" t="s">
         <v>45</v>
-      </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" t="s">
-        <v>48</v>
       </c>
       <c r="M11" t="s">
         <v>28</v>
       </c>
       <c r="N11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" t="s">
-        <v>48</v>
       </c>
       <c r="M12" t="s">
         <v>28</v>
       </c>
       <c r="N12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" t="s">
         <v>44</v>
       </c>
-      <c r="I13" t="s">
+      <c r="L13" t="s">
         <v>45</v>
-      </c>
-      <c r="J13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" t="s">
-        <v>48</v>
       </c>
       <c r="M13" t="s">
         <v>28</v>
       </c>
       <c r="N13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
         <v>44</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>45</v>
-      </c>
-      <c r="J14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" t="s">
-        <v>48</v>
       </c>
       <c r="M14" t="s">
         <v>28</v>
       </c>
       <c r="N14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" t="s">
         <v>44</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
         <v>45</v>
-      </c>
-      <c r="J15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" t="s">
-        <v>48</v>
       </c>
       <c r="M15" t="s">
         <v>28</v>
       </c>
       <c r="N15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
         <v>44</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>45</v>
-      </c>
-      <c r="J16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L16" t="s">
-        <v>48</v>
       </c>
       <c r="M16" t="s">
         <v>28</v>
       </c>
       <c r="N16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" t="s">
         <v>44</v>
       </c>
-      <c r="I17" t="s">
+      <c r="L17" t="s">
         <v>45</v>
-      </c>
-      <c r="J17" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" t="s">
-        <v>47</v>
-      </c>
-      <c r="L17" t="s">
-        <v>48</v>
       </c>
       <c r="M17" t="s">
         <v>28</v>
       </c>
       <c r="N17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>1</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" t="s">
         <v>44</v>
       </c>
-      <c r="I18" t="s">
+      <c r="L18" t="s">
         <v>45</v>
-      </c>
-      <c r="J18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" t="s">
-        <v>48</v>
       </c>
       <c r="M18" t="s">
         <v>28</v>
       </c>
       <c r="N18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
         <v>73</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1861,117 +1919,102 @@
         <v>74</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" t="s">
         <v>75</v>
       </c>
       <c r="I20" t="s">
         <v>76</v>
+      </c>
+      <c r="J20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s">
+        <v>78</v>
+      </c>
+      <c r="L20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O20" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="H21" t="s">
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="K21" t="s">
-        <v>81</v>
-      </c>
-      <c r="L21" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="L21">
+        <v>3320</v>
       </c>
       <c r="M21" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="N21" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="O21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22" t="s">
         <v>90</v>
       </c>
-      <c r="L22">
-        <v>3320</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="P21" t="s">
         <v>91</v>
       </c>
-      <c r="N22" t="s">
+      <c r="Q21" t="s">
         <v>92</v>
       </c>
-      <c r="O22" t="s">
+      <c r="R21" t="s">
         <v>93</v>
       </c>
-      <c r="P22" t="s">
+      <c r="S21" t="s">
         <v>94</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="T21" t="s">
         <v>95</v>
       </c>
-      <c r="R22" t="s">
+      <c r="U21" t="s">
         <v>96</v>
-      </c>
-      <c r="S22" t="s">
-        <v>97</v>
-      </c>
-      <c r="T22" t="s">
-        <v>98</v>
-      </c>
-      <c r="U22" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E22">
+  <conditionalFormatting sqref="E2:E21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>